<commit_message>
Changed to support, motor car, three wheelers, trucks and lorry
</commit_message>
<xml_diff>
--- a/src/main/java/lk/allianz/emotor/resources/smoke_test_data_sheet.xlsx
+++ b/src/main/java/lk/allianz/emotor/resources/smoke_test_data_sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="testcase_1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="153">
   <si>
     <t>customer</t>
   </si>
@@ -469,6 +469,15 @@
   </si>
   <si>
     <t>AUDI</t>
+  </si>
+  <si>
+    <t>BAY-1212</t>
+  </si>
+  <si>
+    <t>LB-4532</t>
+  </si>
+  <si>
+    <t>AAB-9602</t>
   </si>
 </sst>
 </file>
@@ -825,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="Z4" sqref="Z4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="15"/>
@@ -1026,7 +1035,7 @@
         <v>31</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>102</v>
+        <v>150</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>49</v>
@@ -1094,7 +1103,7 @@
         <v>31</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>55</v>
+        <v>151</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>49</v>
@@ -1162,7 +1171,7 @@
         <v>31</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>54</v>
+        <v>152</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>37</v>
@@ -2716,7 +2725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AB2" sqref="AB2:AB8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
regression test to check premiums and quotation and covernote
</commit_message>
<xml_diff>
--- a/src/main/java/lk/allianz/emotor/resources/smoke_test_data_sheet.xlsx
+++ b/src/main/java/lk/allianz/emotor/resources/smoke_test_data_sheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="156">
   <si>
     <t>customer</t>
   </si>
@@ -478,6 +478,15 @@
   </si>
   <si>
     <t>AAB-9602</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>aaaaa</t>
+  </si>
+  <si>
+    <t>dfdfdef</t>
   </si>
 </sst>
 </file>
@@ -832,626 +841,638 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z9"/>
+  <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="10" width="18.28515625" style="1"/>
-    <col min="11" max="11" width="18.28515625" style="3"/>
-    <col min="12" max="18" width="18.28515625" style="1"/>
-    <col min="19" max="19" width="18.28515625" style="3"/>
-    <col min="20" max="20" width="18.28515625" style="1"/>
-    <col min="21" max="21" width="29.85546875" style="1" customWidth="1"/>
-    <col min="22" max="24" width="18.28515625" style="3"/>
-    <col min="25" max="25" width="30.7109375" style="1" customWidth="1"/>
-    <col min="26" max="26" width="75.7109375" style="1" customWidth="1"/>
-    <col min="27" max="16384" width="18.28515625" style="1"/>
+    <col min="1" max="11" width="18.28515625" style="1"/>
+    <col min="12" max="12" width="18.28515625" style="3"/>
+    <col min="13" max="19" width="18.28515625" style="1"/>
+    <col min="20" max="20" width="18.28515625" style="3"/>
+    <col min="21" max="21" width="18.28515625" style="1"/>
+    <col min="22" max="22" width="29.85546875" style="1" customWidth="1"/>
+    <col min="23" max="25" width="18.28515625" style="3"/>
+    <col min="26" max="26" width="30.7109375" style="1" customWidth="1"/>
+    <col min="27" max="27" width="75.7109375" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="18.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="4" customFormat="1">
+    <row r="1" spans="1:27" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
-      <c r="A2" s="1">
+    <row r="2" spans="1:27">
+      <c r="A2" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="R2" s="2">
+      <c r="S2" s="2">
         <v>2307000</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="30">
-      <c r="A3" s="1">
+    <row r="3" spans="1:27" ht="30">
+      <c r="A3" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="R3" s="2">
+      <c r="S3" s="2">
         <v>2400000</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="Z3" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="Z3" s="1" t="s">
+      <c r="AA3" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
-      <c r="A4" s="1">
+    <row r="4" spans="1:27">
+      <c r="A4" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="R4" s="2">
+      <c r="S4" s="2">
         <v>1000000</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="U4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="V4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="X4" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="Y4" s="1" t="s">
+      <c r="Z4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Z4" s="1" t="s">
+      <c r="AA4" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
-      <c r="A5" s="1">
+    <row r="5" spans="1:27">
+      <c r="B5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="L5" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="R5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="R5" s="2">
+      <c r="S5" s="2">
         <v>1200000</v>
       </c>
-      <c r="S5" s="3" t="s">
+      <c r="T5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="U5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="V5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="V5" s="3" t="s">
+      <c r="W5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="W5" s="3" t="s">
+      <c r="X5" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="X5" s="3" t="s">
+      <c r="Y5" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="Y5" s="1" t="s">
+      <c r="Z5" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="Z5" s="1" t="s">
+      <c r="AA5" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
-      <c r="B6" s="1" t="s">
+    <row r="6" spans="1:27">
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="Q6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="R6" s="2">
+      <c r="S6" s="2">
         <v>1200000</v>
       </c>
-      <c r="S6" s="3" t="s">
+      <c r="T6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="U6" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="V6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="V6" s="3" t="s">
+      <c r="W6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="W6" s="3" t="s">
+      <c r="X6" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="X6" s="3" t="s">
+      <c r="Y6" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="Y6" s="1" t="s">
+      <c r="Z6" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="Z6" s="1" t="s">
+      <c r="AA6" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
-      <c r="B7" s="1" t="s">
+    <row r="7" spans="1:27">
+      <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="L7" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="R7" s="2">
+      <c r="S7" s="2">
         <v>1200000</v>
       </c>
-      <c r="S7" s="3" t="s">
+      <c r="T7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="U7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="U7" s="1" t="s">
+      <c r="V7" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="V7" s="3" t="s">
+      <c r="W7" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="W7" s="3" t="s">
+      <c r="X7" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="X7" s="3" t="s">
+      <c r="Y7" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="Y7" s="1" t="s">
+      <c r="Z7" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
-      <c r="B8" s="1" t="s">
+    <row r="8" spans="1:27">
+      <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="L8" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="P8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="Q8" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="R8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="R8" s="2">
+      <c r="S8" s="2">
         <v>1200000</v>
       </c>
-      <c r="S8" s="3" t="s">
+      <c r="T8" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="T8" s="1" t="s">
+      <c r="U8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="U8" s="1" t="s">
+      <c r="V8" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="V8" s="3" t="s">
+      <c r="W8" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="W8" s="3" t="s">
+      <c r="X8" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="X8" s="3" t="s">
+      <c r="Y8" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="Y8" s="1" t="s">
+      <c r="Z8" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
-      <c r="B9" s="1" t="s">
+    <row r="9" spans="1:27">
+      <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="L9" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="P9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="Q9" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="R9" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="R9" s="2">
+      <c r="S9" s="2">
         <v>1200000</v>
       </c>
-      <c r="S9" s="3" t="s">
+      <c r="T9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="U9" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="U9" s="1" t="s">
+      <c r="V9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="V9" s="3" t="s">
+      <c r="W9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="W9" s="3" t="s">
+      <c r="X9" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="X9" s="3" t="s">
+      <c r="Y9" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="Y9" s="1" t="s">
+      <c r="Z9" s="1" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1466,7 +1487,7 @@
   <dimension ref="A1:AE9"/>
   <sheetViews>
     <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:V1048576"/>
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="15"/>

</xml_diff>